<commit_message>
Updated sheet to contain data on companies and where they operate
</commit_message>
<xml_diff>
--- a/Documentation/TariffData.xlsx
+++ b/Documentation/TariffData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tariff Costs" sheetId="1" r:id="rId1"/>
+    <sheet name="Supplier" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -70,13 +70,193 @@
   </si>
   <si>
     <t>Energex</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>http://www.australianpowerandgas.com.au/</t>
+  </si>
+  <si>
+    <t>http://www.originenergy.com.au/962/Energy-Price-Fact-Sheets</t>
+  </si>
+  <si>
+    <t>http://www.energex.com.au/</t>
+  </si>
+  <si>
+    <t>http://www.switchwise.com.au/electricity/sydney-nsw/</t>
+  </si>
+  <si>
+    <t>Suppliers</t>
+  </si>
+  <si>
+    <t>Australian Power and Gas</t>
+  </si>
+  <si>
+    <t>http://www.truenergy.com.au/index.xhtml</t>
+  </si>
+  <si>
+    <t>TRU Energy</t>
+  </si>
+  <si>
+    <t>Actew Agl</t>
+  </si>
+  <si>
+    <t>http://www.actewagl.com.au/</t>
+  </si>
+  <si>
+    <t>http://www.agl.com.au/</t>
+  </si>
+  <si>
+    <t>AGL</t>
+  </si>
+  <si>
+    <t>http://www.alintadirect.com.au/?AspxAutoDetectCookieSupport=1</t>
+  </si>
+  <si>
+    <t>Alinta Direct</t>
+  </si>
+  <si>
+    <t>http://www.auroraenergy.com.au/</t>
+  </si>
+  <si>
+    <t>Aurora Energy</t>
+  </si>
+  <si>
+    <t>http://www.clickenergy.com.au/</t>
+  </si>
+  <si>
+    <t>Click Energy</t>
+  </si>
+  <si>
+    <t>http://www.countryenergy.com.au/</t>
+  </si>
+  <si>
+    <t>Country Energy</t>
+  </si>
+  <si>
+    <t>http://diamondenergy.com.au/home/</t>
+  </si>
+  <si>
+    <t>Diamond Energy</t>
+  </si>
+  <si>
+    <t>http://www.dodo.com/</t>
+  </si>
+  <si>
+    <t>Dodo</t>
+  </si>
+  <si>
+    <t>http://www.energyaustralia.com.au/</t>
+  </si>
+  <si>
+    <t>Energy Australia</t>
+  </si>
+  <si>
+    <t>http://www.ergon.com.au/</t>
+  </si>
+  <si>
+    <t>Ergon</t>
+  </si>
+  <si>
+    <t>http://www.horizonpower.com.au/</t>
+  </si>
+  <si>
+    <t>Horizon Power</t>
+  </si>
+  <si>
+    <t>http://www.integral.com.au/wps/wcm/connect/IE/home/home</t>
+  </si>
+  <si>
+    <t>Integral Energy</t>
+  </si>
+  <si>
+    <t>Jackgreen Energy</t>
+  </si>
+  <si>
+    <t>http://www.lumoenergy.com.au/</t>
+  </si>
+  <si>
+    <t>Lumo Energy</t>
+  </si>
+  <si>
+    <t>Momentum Energy</t>
+  </si>
+  <si>
+    <t>http://www.momentumenergy.com.au/</t>
+  </si>
+  <si>
+    <t>http://www.neighbourhood.com.au/</t>
+  </si>
+  <si>
+    <t>Neighbour Hood</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>http://www.powerwater.com.au/</t>
+  </si>
+  <si>
+    <t>Power Water</t>
+  </si>
+  <si>
+    <t>Power Direct</t>
+  </si>
+  <si>
+    <t>http://www.powerdirect.com.au/</t>
+  </si>
+  <si>
+    <t>http://www.qenergy.com.au/</t>
+  </si>
+  <si>
+    <t>Qenergy</t>
+  </si>
+  <si>
+    <t>http://www.lumoenergy.com.au/your-home-energy</t>
+  </si>
+  <si>
+    <t>Queensland Energy</t>
+  </si>
+  <si>
+    <t>Red Energy</t>
+  </si>
+  <si>
+    <t>http://www.switchwise.com.au/electricity/suppliers/red-energy/</t>
+  </si>
+  <si>
+    <t>Simple Energy</t>
+  </si>
+  <si>
+    <t>http://www.simplyenergy.com.au/</t>
+  </si>
+  <si>
+    <t>South Australia Energy</t>
+  </si>
+  <si>
+    <t>http://www.southaustraliaelectricity.com.au/</t>
+  </si>
+  <si>
+    <t>SYNERGY</t>
+  </si>
+  <si>
+    <t>http://www.synergy.net.au/index.xhtml</t>
+  </si>
+  <si>
+    <t>http://www.victoriaelectricity.com.au/</t>
+  </si>
+  <si>
+    <t>Victoria Energy</t>
+  </si>
+  <si>
+    <t>DATA NOT FOUND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +272,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +307,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,10 +338,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -127,12 +350,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -430,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,12 +886,1681 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K349"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="75.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A30" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="10"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="10"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="2"/>
+      <c r="C54" s="10"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="2"/>
+      <c r="C56" s="10"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+      <c r="C57" s="10"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="C60" s="10"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="10"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="C62" s="10"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="C63" s="10"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="C64" s="10"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+      <c r="C65" s="10"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="C66" s="10"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+      <c r="C67" s="10"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="2"/>
+      <c r="C68" s="10"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="10"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="C70" s="10"/>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="C72" s="10"/>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="C74" s="10"/>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+      <c r="C75" s="10"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="C77" s="10"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="C78" s="10"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="10"/>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="C80" s="10"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="10"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="10"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+      <c r="C83" s="10"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="C84" s="10"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="C85" s="10"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="10"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="C87" s="10"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="10"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="10"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="10"/>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="2"/>
+      <c r="C91" s="10"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+      <c r="C92" s="10"/>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="10"/>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="10"/>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="2"/>
+      <c r="C95" s="10"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="2"/>
+      <c r="C96" s="10"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="2"/>
+      <c r="C97" s="10"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+      <c r="C98" s="10"/>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="2"/>
+      <c r="C99" s="10"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="2"/>
+      <c r="C100" s="10"/>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="2"/>
+      <c r="C101" s="10"/>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+      <c r="C102" s="10"/>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="2"/>
+      <c r="C103" s="10"/>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="2"/>
+      <c r="C104" s="10"/>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="2"/>
+      <c r="C105" s="10"/>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="2"/>
+      <c r="C106" s="10"/>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="2"/>
+      <c r="C107" s="10"/>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="2"/>
+      <c r="C108" s="10"/>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="2"/>
+      <c r="C109" s="10"/>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="2"/>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="2"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="2"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="2"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="2"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="2"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="2"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="2"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="2"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="2"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="2"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="2"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="2"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="2"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="2"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" s="2"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="2"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="2"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="2"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="2"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="2"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="2"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="2"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="2"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="2"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" s="2"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="2"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" s="2"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="2"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165" s="2"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="2"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169" s="2"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170" s="2"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171" s="2"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" s="2"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B174" s="2"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175" s="2"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="2"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179" s="2"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180" s="2"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181" s="2"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182" s="2"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B183" s="2"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B184" s="2"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B185" s="2"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186" s="2"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187" s="2"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188" s="2"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B189" s="2"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190" s="2"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191" s="2"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192" s="2"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194" s="2"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B196" s="2"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B197" s="2"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B198" s="2"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200" s="2"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B201" s="2"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202" s="2"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B203" s="2"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B205" s="2"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B206" s="2"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B207" s="2"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B208" s="2"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B209" s="2"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B210" s="2"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B216" s="2"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B217" s="2"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B218" s="2"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B219" s="2"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B220" s="2"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B221" s="2"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B222" s="2"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B223" s="2"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B224" s="2"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B225" s="2"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B226" s="2"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B227" s="2"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B228" s="2"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B229" s="2"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B232" s="2"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B235" s="2"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B236" s="2"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B237" s="2"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B239" s="2"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B240" s="2"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241" s="2"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242" s="2"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B244" s="2"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B245" s="2"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B246" s="2"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B248" s="2"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B249" s="2"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B250" s="2"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B251" s="2"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B252" s="2"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B253" s="2"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B254" s="2"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B255" s="2"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B256" s="2"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B257" s="2"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B258" s="2"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B259" s="2"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B260" s="2"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B261" s="2"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B262" s="2"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B263" s="2"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B264" s="2"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B265" s="2"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B266" s="2"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B267" s="2"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B268" s="2"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B269" s="2"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B270" s="2"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B271" s="2"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B272" s="2"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B273" s="2"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B274" s="2"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B275" s="2"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B276" s="2"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B277" s="2"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B278" s="2"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B279" s="2"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B280" s="2"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B281" s="2"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B282" s="2"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B283" s="2"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B284" s="2"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B285" s="2"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B286" s="2"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B287" s="2"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B288" s="2"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B289" s="2"/>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B290" s="2"/>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B291" s="2"/>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B292" s="2"/>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B293" s="2"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B294" s="2"/>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B295" s="2"/>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B296" s="2"/>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B297" s="2"/>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B298" s="2"/>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B299" s="2"/>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B300" s="2"/>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B301" s="2"/>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B302" s="2"/>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B303" s="2"/>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B304" s="2"/>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B305" s="2"/>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B306" s="2"/>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B307" s="2"/>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B308" s="2"/>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B309" s="2"/>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B310" s="2"/>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B311" s="2"/>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B312" s="2"/>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B313" s="2"/>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B314" s="2"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B315" s="2"/>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B316" s="2"/>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B317" s="2"/>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B318" s="2"/>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B319" s="2"/>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B320" s="2"/>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B321" s="2"/>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B322" s="2"/>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B323" s="2"/>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B324" s="2"/>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B325" s="2"/>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B326" s="2"/>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B327" s="2"/>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B328" s="2"/>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B329" s="2"/>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B330" s="2"/>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B331" s="2"/>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B332" s="2"/>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B333" s="2"/>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B334" s="2"/>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B335" s="2"/>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B336" s="2"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B337" s="2"/>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B338" s="2"/>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B339" s="2"/>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B340" s="2"/>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B341" s="2"/>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B342" s="2"/>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B343" s="2"/>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B344" s="2"/>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B345" s="2"/>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B346" s="2"/>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B347" s="2"/>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B348" s="2"/>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B349" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="A32" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C6" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changed loading of Tariffs so it only occurs on initial load.
</commit_message>
<xml_diff>
--- a/Documentation/TariffData.xlsx
+++ b/Documentation/TariffData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -349,6 +349,21 @@
   </si>
   <si>
     <t>http://www.australianpowerandgas.com.au/documents/PriceDocuments/Electricity/OriginCP_GDGR.pdf</t>
+  </si>
+  <si>
+    <t>http://www.originenergy.com.au/priceguide/?_qf_p2_display=true&amp;ga_vs=http%3A%2F%2Fwww.originenergy.com.au%2F</t>
+  </si>
+  <si>
+    <t>http://www.originenergy.com.au/2716/Feed-in-tariffs</t>
+  </si>
+  <si>
+    <t>http://www.originenergy.com.au/2716/Feed-in-tariffs?g[user_state]=nsw</t>
+  </si>
+  <si>
+    <t>http://www.originenergy.com.au/2716/Feed-in-tariffs?g[user_state]=sa</t>
+  </si>
+  <si>
+    <t>http://www.originenergy.com.au/2716/Feed-in-tariffs?g[user_state]=vic</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1154,8 @@
   <dimension ref="A1:V485"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,15 +1217,15 @@
       </c>
       <c r="R1" s="47">
         <f ca="1">(J234 - P1) / V1</f>
-        <v>7.2727272727272725</v>
+        <v>1.3913043478260869</v>
       </c>
       <c r="U1" s="43">
         <f ca="1">(NOW()-TIME(11,0,0))</f>
-        <v>41179.09203634259</v>
+        <v>41191.479418055555</v>
       </c>
       <c r="V1" s="44">
         <f ca="1">HOUR(U1) + MINUTE(U1) / 60</f>
-        <v>2.2000000000000002</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1326,11 +1341,11 @@
         <v>-</v>
       </c>
       <c r="F4" s="10" t="str">
-        <f t="shared" ref="F4:F12" ca="1" si="3">IF(C4 = ".", "-","" )</f>
+        <f t="shared" ref="F4:F8" ca="1" si="3">IF(C4 = ".", "-","" )</f>
         <v>-</v>
       </c>
       <c r="G4" s="10" t="str">
-        <f t="shared" ref="G4:G12" ca="1" si="4">IF(C4 = ".", "-","" )</f>
+        <f t="shared" ref="G4:G8" ca="1" si="4">IF(C4 = ".", "-","" )</f>
         <v>-</v>
       </c>
       <c r="H4" s="31" t="str">
@@ -1845,11 +1860,11 @@
         <v>-</v>
       </c>
       <c r="F15" s="10" t="str">
-        <f t="shared" ref="F14:F77" ca="1" si="6">IF(C15 = ".", "-","" )</f>
+        <f t="shared" ref="F15:F77" ca="1" si="6">IF(C15 = ".", "-","" )</f>
         <v>-</v>
       </c>
       <c r="G15" s="10" t="str">
-        <f t="shared" ref="G14:G77" ca="1" si="7">IF(C15 = ".", "-","" )</f>
+        <f t="shared" ref="G15:G77" ca="1" si="7">IF(C15 = ".", "-","" )</f>
         <v>-</v>
       </c>
       <c r="H15" s="31" t="str">
@@ -8446,25 +8461,20 @@
         <f t="shared" ref="C138" ca="1" si="274">IF(INDIRECT("Supplier!D"&amp;(FLOOR((CELL("row",A138)-2)/8,1)+1)+1)&lt;&gt;"N",INDIRECT("Supplier!D1"),".")</f>
         <v>QLD</v>
       </c>
-      <c r="D138" s="10" t="str">
-        <f t="shared" ca="1" si="258"/>
-        <v/>
-      </c>
-      <c r="E138" s="10" t="str">
-        <f t="shared" ca="1" si="223"/>
-        <v/>
-      </c>
-      <c r="F138" s="10" t="str">
-        <f t="shared" ca="1" si="144"/>
-        <v/>
-      </c>
-      <c r="G138" s="10" t="str">
-        <f t="shared" ca="1" si="145"/>
-        <v/>
-      </c>
-      <c r="H138" s="31" t="str">
-        <f t="shared" ca="1" si="224"/>
-        <v/>
+      <c r="D138" s="10">
+        <v>25.3781</v>
+      </c>
+      <c r="E138" s="10">
+        <v>12.1099</v>
+      </c>
+      <c r="F138" s="10">
+        <v>28.786999999999999</v>
+      </c>
+      <c r="G138" s="10">
+        <v>28.786999999999999</v>
+      </c>
+      <c r="H138" s="31">
+        <v>8</v>
       </c>
       <c r="I138">
         <f t="shared" ca="1" si="262"/>
@@ -8475,13 +8485,13 @@
         <v>1</v>
       </c>
       <c r="K138" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="L138" s="53" t="s">
         <v>78</v>
       </c>
       <c r="M138" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="N138" t="s">
         <v>78</v>
@@ -8500,25 +8510,20 @@
         <f t="shared" ref="C139" ca="1" si="276">IF(INDIRECT("Supplier!E"&amp;(FLOOR((CELL("row",A139)-2)/8,1)+1)+1)&lt;&gt;"N",INDIRECT("Supplier!E1"),".")</f>
         <v>NSW</v>
       </c>
-      <c r="D139" s="10" t="str">
-        <f t="shared" ca="1" si="258"/>
-        <v/>
-      </c>
-      <c r="E139" s="10" t="str">
-        <f t="shared" ca="1" si="223"/>
-        <v/>
-      </c>
-      <c r="F139" s="10" t="str">
-        <f t="shared" ca="1" si="144"/>
-        <v/>
-      </c>
-      <c r="G139" s="10" t="str">
-        <f t="shared" ca="1" si="145"/>
-        <v/>
-      </c>
-      <c r="H139" s="31" t="str">
-        <f t="shared" ca="1" si="224"/>
-        <v/>
+      <c r="D139" s="10">
+        <v>28.05</v>
+      </c>
+      <c r="E139" s="10">
+        <v>11.11</v>
+      </c>
+      <c r="F139" s="10">
+        <v>69.08</v>
+      </c>
+      <c r="G139" s="10">
+        <v>69.08</v>
+      </c>
+      <c r="H139" s="31">
+        <v>6</v>
       </c>
       <c r="I139">
         <f t="shared" ca="1" si="262"/>
@@ -8529,13 +8534,13 @@
         <v>1</v>
       </c>
       <c r="K139" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="L139" s="53" t="s">
         <v>78</v>
       </c>
       <c r="M139" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="N139" t="s">
         <v>78</v>
@@ -8554,25 +8559,20 @@
         <f t="shared" ref="C140" ca="1" si="278">IF(INDIRECT("Supplier!F"&amp;(FLOOR((CELL("row",A140)-2)/8,1)+1)+1)&lt;&gt;"N",INDIRECT("Supplier!F1"),".")</f>
         <v>VIC</v>
       </c>
-      <c r="D140" s="10" t="str">
-        <f t="shared" ca="1" si="258"/>
-        <v/>
-      </c>
-      <c r="E140" s="10" t="str">
-        <f t="shared" ca="1" si="223"/>
-        <v/>
-      </c>
-      <c r="F140" s="10" t="str">
-        <f t="shared" ca="1" si="144"/>
-        <v/>
-      </c>
-      <c r="G140" s="10" t="str">
-        <f t="shared" ca="1" si="145"/>
-        <v/>
-      </c>
-      <c r="H140" s="31" t="str">
-        <f t="shared" ca="1" si="224"/>
-        <v/>
+      <c r="D140" s="10">
+        <v>23.199000000000002</v>
+      </c>
+      <c r="E140" s="10">
+        <v>12.188000000000001</v>
+      </c>
+      <c r="F140" s="10">
+        <v>85.88</v>
+      </c>
+      <c r="G140" s="10">
+        <v>85.88</v>
+      </c>
+      <c r="H140" s="31">
+        <v>8</v>
       </c>
       <c r="I140">
         <f t="shared" ca="1" si="262"/>
@@ -8583,13 +8583,13 @@
         <v>1</v>
       </c>
       <c r="K140" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="L140" s="53" t="s">
         <v>78</v>
       </c>
       <c r="M140" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="N140" t="s">
         <v>78</v>
@@ -8662,25 +8662,20 @@
         <f t="shared" ref="C142" ca="1" si="282">IF(INDIRECT("Supplier!H"&amp;(FLOOR((CELL("row",A142)-2)/8,1)+1)+1)&lt;&gt;"N",INDIRECT("Supplier!H1"),".")</f>
         <v>SA</v>
       </c>
-      <c r="D142" s="10" t="str">
-        <f t="shared" ca="1" si="258"/>
-        <v/>
-      </c>
-      <c r="E142" s="10" t="str">
-        <f t="shared" ca="1" si="223"/>
-        <v/>
-      </c>
-      <c r="F142" s="10" t="str">
-        <f t="shared" ref="F142:F205" ca="1" si="283">IF(C142 = ".", "-","" )</f>
-        <v/>
-      </c>
-      <c r="G142" s="10" t="str">
-        <f t="shared" ref="G142:G205" ca="1" si="284">IF(C142 = ".", "-","" )</f>
-        <v/>
-      </c>
-      <c r="H142" s="31" t="str">
-        <f t="shared" ca="1" si="224"/>
-        <v/>
+      <c r="D142" s="10">
+        <v>34</v>
+      </c>
+      <c r="E142" s="10">
+        <v>16.14</v>
+      </c>
+      <c r="F142" s="10">
+        <v>75.152000000000001</v>
+      </c>
+      <c r="G142" s="10">
+        <v>75.152000000000001</v>
+      </c>
+      <c r="H142" s="31">
+        <v>9.8000000000000007</v>
       </c>
       <c r="I142">
         <f t="shared" ca="1" si="262"/>
@@ -8691,13 +8686,13 @@
         <v>1</v>
       </c>
       <c r="K142" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="L142" s="53" t="s">
         <v>78</v>
       </c>
       <c r="M142" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="N142" t="s">
         <v>78</v>
@@ -8709,11 +8704,11 @@
         <v>18</v>
       </c>
       <c r="B143" s="12" t="str">
-        <f t="shared" ref="B143" ca="1" si="285">B138</f>
+        <f t="shared" ref="B143" ca="1" si="283">B138</f>
         <v>Origin</v>
       </c>
       <c r="C143" s="12" t="str">
-        <f t="shared" ref="C143" ca="1" si="286">IF(INDIRECT("Supplier!I"&amp;(FLOOR((CELL("row",A143)-2)/8,1)+1)+1)&lt;&gt;"N",INDIRECT("Supplier!I1"),".")</f>
+        <f t="shared" ref="C143" ca="1" si="284">IF(INDIRECT("Supplier!I"&amp;(FLOOR((CELL("row",A143)-2)/8,1)+1)+1)&lt;&gt;"N",INDIRECT("Supplier!I1"),".")</f>
         <v>.</v>
       </c>
       <c r="D143" s="10" t="str">
@@ -8725,11 +8720,11 @@
         <v>-</v>
       </c>
       <c r="F143" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ref="F142:F205" ca="1" si="285">IF(C143 = ".", "-","" )</f>
         <v>-</v>
       </c>
       <c r="G143" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ref="G142:G205" ca="1" si="286">IF(C143 = ".", "-","" )</f>
         <v>-</v>
       </c>
       <c r="H143" s="31" t="str">
@@ -8779,11 +8774,11 @@
         <v>-</v>
       </c>
       <c r="F144" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G144" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H144" s="31" t="str">
@@ -8833,11 +8828,11 @@
         <v>-</v>
       </c>
       <c r="F145" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G145" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H145" s="31" t="str">
@@ -8887,11 +8882,11 @@
         <v>-</v>
       </c>
       <c r="F146" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G146" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H146" s="31" t="str">
@@ -8941,11 +8936,11 @@
         <v>-</v>
       </c>
       <c r="F147" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G147" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H147" s="31" t="str">
@@ -8995,11 +8990,11 @@
         <v>-</v>
       </c>
       <c r="F148" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G148" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H148" s="31" t="str">
@@ -9049,11 +9044,11 @@
         <v>-</v>
       </c>
       <c r="F149" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G149" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H149" s="31" t="str">
@@ -9103,11 +9098,11 @@
         <v>-</v>
       </c>
       <c r="F150" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G150" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H150" s="31" t="str">
@@ -9206,11 +9201,11 @@
         <v>-</v>
       </c>
       <c r="F152" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G152" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H152" s="31" t="str">
@@ -9260,11 +9255,11 @@
         <v>-</v>
       </c>
       <c r="F153" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G153" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H153" s="31" t="str">
@@ -9314,11 +9309,11 @@
         <v/>
       </c>
       <c r="F154" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G154" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H154" s="31" t="str">
@@ -9368,11 +9363,11 @@
         <v/>
       </c>
       <c r="F155" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G155" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H155" s="31" t="str">
@@ -9422,11 +9417,11 @@
         <v/>
       </c>
       <c r="F156" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G156" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H156" s="31" t="str">
@@ -9476,11 +9471,11 @@
         <v>-</v>
       </c>
       <c r="F157" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G157" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H157" s="31" t="str">
@@ -9530,11 +9525,11 @@
         <v/>
       </c>
       <c r="F158" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G158" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H158" s="31" t="str">
@@ -9584,11 +9579,11 @@
         <v>-</v>
       </c>
       <c r="F159" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G159" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H159" s="31" t="str">
@@ -9638,11 +9633,11 @@
         <v>-</v>
       </c>
       <c r="F160" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G160" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H160" s="31" t="str">
@@ -9692,11 +9687,11 @@
         <v>-</v>
       </c>
       <c r="F161" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G161" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H161" s="31" t="str">
@@ -9746,11 +9741,11 @@
         <v/>
       </c>
       <c r="F162" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G162" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H162" s="31" t="str">
@@ -9800,11 +9795,11 @@
         <v>-</v>
       </c>
       <c r="F163" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G163" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H163" s="31" t="str">
@@ -9854,11 +9849,11 @@
         <v>-</v>
       </c>
       <c r="F164" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G164" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H164" s="31" t="str">
@@ -9908,11 +9903,11 @@
         <v>-</v>
       </c>
       <c r="F165" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G165" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H165" s="31" t="str">
@@ -9962,11 +9957,11 @@
         <v>-</v>
       </c>
       <c r="F166" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G166" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H166" s="31" t="str">
@@ -10016,11 +10011,11 @@
         <v>-</v>
       </c>
       <c r="F167" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G167" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H167" s="31" t="str">
@@ -10070,11 +10065,11 @@
         <v>-</v>
       </c>
       <c r="F168" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G168" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H168" s="31" t="str">
@@ -10124,11 +10119,11 @@
         <v>-</v>
       </c>
       <c r="F169" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G169" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H169" s="31" t="str">
@@ -10178,11 +10173,11 @@
         <v/>
       </c>
       <c r="F170" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G170" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H170" s="31" t="str">
@@ -10232,11 +10227,11 @@
         <v/>
       </c>
       <c r="F171" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G171" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H171" s="31" t="str">
@@ -10286,11 +10281,11 @@
         <v/>
       </c>
       <c r="F172" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G172" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H172" s="31" t="str">
@@ -10340,11 +10335,11 @@
         <v>-</v>
       </c>
       <c r="F173" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G173" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H173" s="31" t="str">
@@ -10394,11 +10389,11 @@
         <v/>
       </c>
       <c r="F174" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G174" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H174" s="31" t="str">
@@ -10448,11 +10443,11 @@
         <v>-</v>
       </c>
       <c r="F175" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G175" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H175" s="31" t="str">
@@ -10502,11 +10497,11 @@
         <v>-</v>
       </c>
       <c r="F176" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G176" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H176" s="31" t="str">
@@ -10556,11 +10551,11 @@
         <v>-</v>
       </c>
       <c r="F177" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G177" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H177" s="31" t="str">
@@ -10610,11 +10605,11 @@
         <v>-</v>
       </c>
       <c r="F178" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G178" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H178" s="31" t="str">
@@ -10664,11 +10659,11 @@
         <v/>
       </c>
       <c r="F179" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G179" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H179" s="31" t="str">
@@ -10718,11 +10713,11 @@
         <v/>
       </c>
       <c r="F180" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G180" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H180" s="31" t="str">
@@ -10772,11 +10767,11 @@
         <v>-</v>
       </c>
       <c r="F181" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G181" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H181" s="31" t="str">
@@ -10826,11 +10821,11 @@
         <v/>
       </c>
       <c r="F182" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G182" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H182" s="31" t="str">
@@ -10880,11 +10875,11 @@
         <v>-</v>
       </c>
       <c r="F183" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G183" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H183" s="31" t="str">
@@ -10934,11 +10929,11 @@
         <v>-</v>
       </c>
       <c r="F184" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G184" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H184" s="31" t="str">
@@ -10988,11 +10983,11 @@
         <v>-</v>
       </c>
       <c r="F185" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G185" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H185" s="31" t="str">
@@ -11042,11 +11037,11 @@
         <v>-</v>
       </c>
       <c r="F186" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G186" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H186" s="31" t="str">
@@ -11096,11 +11091,11 @@
         <v>-</v>
       </c>
       <c r="F187" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G187" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H187" s="31" t="str">
@@ -11150,11 +11145,11 @@
         <v/>
       </c>
       <c r="F188" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G188" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H188" s="31" t="str">
@@ -11204,11 +11199,11 @@
         <v>-</v>
       </c>
       <c r="F189" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G189" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H189" s="31" t="str">
@@ -11258,11 +11253,11 @@
         <v/>
       </c>
       <c r="F190" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v/>
       </c>
       <c r="G190" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v/>
       </c>
       <c r="H190" s="31" t="str">
@@ -11312,11 +11307,11 @@
         <v>-</v>
       </c>
       <c r="F191" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G191" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H191" s="31" t="str">
@@ -11366,11 +11361,11 @@
         <v>-</v>
       </c>
       <c r="F192" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G192" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H192" s="31" t="str">
@@ -11420,11 +11415,11 @@
         <v>-</v>
       </c>
       <c r="F193" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G193" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H193" s="31" t="str">
@@ -11474,11 +11469,11 @@
         <v>-</v>
       </c>
       <c r="F194" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G194" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H194" s="31" t="str">
@@ -11528,11 +11523,11 @@
         <v>-</v>
       </c>
       <c r="F195" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G195" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H195" s="31" t="str">
@@ -11582,11 +11577,11 @@
         <v>-</v>
       </c>
       <c r="F196" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G196" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H196" s="31" t="str">
@@ -11636,11 +11631,11 @@
         <v>-</v>
       </c>
       <c r="F197" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G197" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H197" s="31" t="str">
@@ -11738,11 +11733,11 @@
         <v>-</v>
       </c>
       <c r="F199" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G199" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H199" s="31" t="str">
@@ -11792,11 +11787,11 @@
         <v>-</v>
       </c>
       <c r="F200" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G200" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H200" s="31" t="str">
@@ -11846,11 +11841,11 @@
         <v>-</v>
       </c>
       <c r="F201" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G201" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H201" s="31" t="str">
@@ -11900,11 +11895,11 @@
         <v>-</v>
       </c>
       <c r="F202" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G202" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H202" s="31" t="str">
@@ -11954,11 +11949,11 @@
         <v>-</v>
       </c>
       <c r="F203" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G203" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H203" s="31" t="str">
@@ -12008,11 +12003,11 @@
         <v>-</v>
       </c>
       <c r="F204" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G204" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H204" s="31" t="str">
@@ -12062,11 +12057,11 @@
         <v>-</v>
       </c>
       <c r="F205" s="10" t="str">
-        <f t="shared" ca="1" si="283"/>
+        <f t="shared" ca="1" si="285"/>
         <v>-</v>
       </c>
       <c r="G205" s="10" t="str">
-        <f t="shared" ca="1" si="284"/>
+        <f t="shared" ca="1" si="286"/>
         <v>-</v>
       </c>
       <c r="H205" s="31" t="str">
@@ -16162,7 +16157,7 @@
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1"/>
     <hyperlink ref="K10" r:id="rId2"/>
-    <hyperlink ref="K22"/>
+    <hyperlink ref="K22" display="http://web.alintaenergy.com.au/BecomeCustomer/SelectAPlanPostcode?PostcodeSuburbState=5000-ADELAIDE%2CSA&amp;ProductClassPackage=Electricity&amp;State=SA&amp;Postcode=5000&amp;Suburb=ADELAIDE&amp;IsMoving=False&amp;CutOffDate=09%2F28%2F2012%2000%3A00%3A00&amp;Holidays=System.Collect"/>
     <hyperlink ref="K34" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>